<commit_message>
Clear all cell contents (formats too) in pivot table range upon loading.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -63,21 +63,6 @@
   </x:si>
   <x:si>
     <x:t>SCONE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NumberOfOrdersPercentageOfBearclaw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column Labels</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Row Labels</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(blank)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Grand Total</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -201,42 +186,9 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="13">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -1012,88 +964,14 @@
     <x:col min="3" max="3" width="11.140625" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C1" s="4" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="3" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B2" s="3" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C2" s="6" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="3" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="8" t="n">
-        <x:v>1.20814479638009</x:v>
-      </x:c>
-      <x:c r="C3" s="9" t="n">
-        <x:v>1.20814479638009</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="10" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B4" s="11" t="n">
-        <x:v>1.54977375565611</x:v>
-      </x:c>
-      <x:c r="C4" s="12" t="n">
-        <x:v>1.54977375565611</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="10" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B5" s="11" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C5" s="12" t="n">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="10" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B6" s="11" t="n">
-        <x:v>1.82126696832579</x:v>
-      </x:c>
-      <x:c r="C6" s="12" t="n">
-        <x:v>1.82126696832579</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="10" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B7" s="11" t="n">
-        <x:v>1.70814479638009</x:v>
-      </x:c>
-      <x:c r="C7" s="12" t="n">
-        <x:v>1.70814479638009</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="13" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B8" s="14" t="s"/>
-      <x:c r="C8" s="15" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="7" spans="1:3" x14ac:dyDescent="0.25"/>
+    <x:row r="8" spans="1:3" x14ac:dyDescent="0.25"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Refactor to use as many of existing pivot cache elements as possible.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
@@ -234,11 +234,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" refreshedBy="Francois Botha" refreshedDate="43250.7489599537" refreshedVersion="5" recordCount="16">
   <x:cacheSource type="worksheet">
     <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
-  <x:cacheFields>
+  <x:cacheFields count="6">
     <x:cacheField name="Name">
       <x:sharedItems count="5">
         <x:s v="Croissant"/>
@@ -264,6 +264,11 @@
       <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </x:ext>
+  </x:extLst>
 </x:pivotCacheDefinition>
 </file>
 

</xml_diff>

<commit_message>
Fix error by two pivot with one source #1195 (#1196)
Fix errors regarding multiple pivot tables with single pivot table cache
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
@@ -234,11 +234,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" refreshedBy="Francois Botha" refreshedDate="43250.7489599537" refreshedVersion="5" recordCount="16">
   <x:cacheSource type="worksheet">
     <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
-  <x:cacheFields>
+  <x:cacheFields count="6">
     <x:cacheField name="Name">
       <x:sharedItems count="5">
         <x:s v="Croissant"/>
@@ -264,6 +264,11 @@
       <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </x:ext>
+  </x:extLst>
 </x:pivotCacheDefinition>
 </file>
 

</xml_diff>